<commit_message>
Added the Open Source certification logo for the M2-R4
</commit_message>
<xml_diff>
--- a/AnthC/Doc/Assembly/AnthC M2-R4/Bill of Materials BOM AnthC M2-R4.xlsx
+++ b/AnthC/Doc/Assembly/AnthC M2-R4/Bill of Materials BOM AnthC M2-R4.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IDM\Repositorios\clients\Anthilla\AnthC\AnthC\Doc\Assembly\AnthC M2-R4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EB64EC23-702B-4E7C-8EF9-833AE8EC31BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F25CD12C-E727-4B15-B729-5DF672DF611F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C0C25B29-7581-4A4E-9EEA-CB0C976B4432}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="255">
   <si>
     <t>Reference</t>
   </si>
@@ -804,6 +804,15 @@
   </si>
   <si>
     <t>Bill of Materials (BOM)</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Unit Price</t>
+  </si>
+  <si>
+    <t>Total Price</t>
   </si>
 </sst>
 </file>
@@ -935,17 +944,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -958,30 +980,75 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thick">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -1017,8 +1084,8 @@
       <xdr:rowOff>11207</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>6555442</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>67236</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>165058</xdr:rowOff>
     </xdr:to>
@@ -1075,13 +1142,16 @@
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="1" xr16:uid="{AE2BCE0E-608F-4273-91B3-63ED9F032931}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="11">
-    <queryTableFields count="5">
+  <queryTableRefresh nextId="14" unboundColumnsRight="3">
+    <queryTableFields count="8">
       <queryTableField id="1" name="Reference" tableColumnId="1"/>
       <queryTableField id="2" name="Value" tableColumnId="2"/>
       <queryTableField id="4" name="Footprint" tableColumnId="4"/>
       <queryTableField id="5" name="Qty" tableColumnId="5"/>
       <queryTableField id="8" name="Manufacturer" tableColumnId="8"/>
+      <queryTableField id="11" dataBound="0" tableColumnId="3"/>
+      <queryTableField id="12" dataBound="0" tableColumnId="6"/>
+      <queryTableField id="13" dataBound="0" tableColumnId="7"/>
     </queryTableFields>
     <queryTableDeletedFields count="5">
       <deletedField name="Datasheet"/>
@@ -1095,14 +1165,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BB47F66F-3CDE-43B9-B45D-C23F0F9396B1}" name="BOM___AnthC_M2_R4" displayName="BOM___AnthC_M2_R4" ref="A9:E73" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A9:E73" xr:uid="{BB47F66F-3CDE-43B9-B45D-C23F0F9396B1}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{AA0D1052-BA94-4D98-B6AA-63B2442248D5}" uniqueName="1" name="Reference" queryTableFieldId="1" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{54FD6537-C3A5-44E3-BC80-5A822DD6E5E0}" uniqueName="2" name="Value" queryTableFieldId="2" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{27FC6405-7B84-4D3B-867E-92448CC266EB}" uniqueName="4" name="Footprint" queryTableFieldId="4" dataDxfId="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BB47F66F-3CDE-43B9-B45D-C23F0F9396B1}" name="BOM___AnthC_M2_R4" displayName="BOM___AnthC_M2_R4" ref="A9:H74" tableType="queryTable" totalsRowCount="1">
+  <autoFilter ref="A9:H73" xr:uid="{BB47F66F-3CDE-43B9-B45D-C23F0F9396B1}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{AA0D1052-BA94-4D98-B6AA-63B2442248D5}" uniqueName="1" name="Reference" queryTableFieldId="1" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{54FD6537-C3A5-44E3-BC80-5A822DD6E5E0}" uniqueName="2" name="Value" queryTableFieldId="2" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{27FC6405-7B84-4D3B-867E-92448CC266EB}" uniqueName="4" name="Footprint" queryTableFieldId="4" dataDxfId="6"/>
     <tableColumn id="5" xr3:uid="{6B82F80F-D833-45C1-AD4F-941CF7BC4402}" uniqueName="5" name="Qty" queryTableFieldId="5"/>
-    <tableColumn id="8" xr3:uid="{A2B66114-56B8-4D32-9D60-C20DD972B168}" uniqueName="8" name="Manufacturer" queryTableFieldId="8" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{A2B66114-56B8-4D32-9D60-C20DD972B168}" uniqueName="8" name="Manufacturer" queryTableFieldId="8" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{9BD008AA-1ABC-496D-AE08-E658162E63CB}" uniqueName="3" name="MPN" totalsRowLabel="Total" queryTableFieldId="11" dataDxfId="4" totalsRowDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{D56D72D5-992D-451A-9D46-F868D2147D45}" uniqueName="6" name="Unit Price" queryTableFieldId="12" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{1659BAE1-86FE-4883-81FD-2B8BFF671E0F}" uniqueName="7" name="Total Price" totalsRowFunction="custom" queryTableFieldId="13" dataDxfId="2" totalsRowDxfId="0">
+      <calculatedColumnFormula>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</calculatedColumnFormula>
+      <totalsRowFormula>SUM(H10:H73)</totalsRowFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1425,93 +1501,103 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74FC2818-A30F-4222-AEA1-FF26AF583BC9}">
-  <dimension ref="A1:F74"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:H74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="116.7109375" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="80.28515625" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="57.5703125" customWidth="1"/>
     <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.28515625" customWidth="1"/>
+    <col min="6" max="6" width="31.140625" customWidth="1"/>
+    <col min="7" max="7" width="24.140625" customWidth="1"/>
+    <col min="8" max="8" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
         <v>251</v>
       </c>
-      <c r="B1" s="11"/>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="12"/>
-      <c r="B2" s="13"/>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="16"/>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="17"/>
+      <c r="B2" s="18"/>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="3"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="11" t="s">
         <v>246</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="19" t="s">
         <v>247</v>
       </c>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="15"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="9"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="19" t="s">
         <v>249</v>
       </c>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="15"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="9"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="11" t="s">
         <v>250</v>
       </c>
-      <c r="C6" s="16">
+      <c r="C6" s="20">
         <v>45367</v>
       </c>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="17"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="10"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="6"/>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="9"/>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="6"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="8"/>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -1527,1291 +1613,1805 @@
       <c r="E9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
+      <c r="G9" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="5">
-        <v>1</v>
-      </c>
-      <c r="E10" s="20" t="s">
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="21" t="s">
+      <c r="F10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="19" t="s">
+      <c r="G10" s="21">
+        <v>3.0339999999999998</v>
+      </c>
+      <c r="H10" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>3.0339999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11">
         <v>8</v>
       </c>
-      <c r="E11" s="20" t="s">
+      <c r="E11" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="21" t="s">
+      <c r="F11" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
+      <c r="G11" s="21">
+        <v>2.9899999999999999E-2</v>
+      </c>
+      <c r="H11" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>0.2392</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C12" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="5">
-        <v>1</v>
-      </c>
-      <c r="E12" s="20" t="s">
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
         <v>20</v>
       </c>
-      <c r="F12" s="21" t="s">
+      <c r="F12" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="19" t="s">
+      <c r="G12" s="21">
+        <f>0.0621/20</f>
+        <v>3.1050000000000001E-3</v>
+      </c>
+      <c r="H12" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>3.1050000000000001E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13">
         <v>19</v>
       </c>
-      <c r="E13" s="20" t="s">
+      <c r="E13" t="s">
         <v>20</v>
       </c>
-      <c r="F13" s="21" t="s">
+      <c r="F13" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="19" t="s">
+      <c r="G13" s="21">
+        <f>0.406/196</f>
+        <v>2.0714285714285717E-3</v>
+      </c>
+      <c r="H13" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>3.9357142857142861E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C14" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="5">
-        <v>1</v>
-      </c>
-      <c r="E14" s="20" t="s">
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="21" t="s">
+      <c r="F14" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
+      <c r="G14" s="21">
+        <f>0.1167/20</f>
+        <v>5.8349999999999999E-3</v>
+      </c>
+      <c r="H14" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>5.8349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="C15" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="5">
-        <v>1</v>
-      </c>
-      <c r="E15" s="20" t="s">
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
         <v>31</v>
       </c>
-      <c r="F15" s="21" t="s">
+      <c r="F15" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="19" t="s">
+      <c r="G15" s="21">
+        <f>0.0169/20</f>
+        <v>8.4499999999999994E-4</v>
+      </c>
+      <c r="H15" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>8.4499999999999994E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C16" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16">
         <v>3</v>
       </c>
-      <c r="E16" s="20" t="s">
+      <c r="E16" t="s">
         <v>15</v>
       </c>
-      <c r="F16" s="21" t="s">
+      <c r="F16" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="19" t="s">
+      <c r="G16" s="21">
+        <f>2.121/32</f>
+        <v>6.628125E-2</v>
+      </c>
+      <c r="H16" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>0.19884374999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="B17" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="20" t="s">
+      <c r="C17" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17">
         <v>4</v>
       </c>
-      <c r="E17" s="20" t="s">
+      <c r="E17" t="s">
         <v>20</v>
       </c>
-      <c r="F17" s="21" t="s">
+      <c r="F17" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
+      <c r="G17" s="21">
+        <f>0.2213/50</f>
+        <v>4.4260000000000002E-3</v>
+      </c>
+      <c r="H17" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>1.7704000000000001E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="B18" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C18" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18">
         <v>4</v>
       </c>
-      <c r="E18" s="20" t="s">
+      <c r="E18" t="s">
         <v>20</v>
       </c>
-      <c r="F18" s="21" t="s">
+      <c r="F18" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="19" t="s">
+      <c r="G18" s="21">
+        <f>0.0996/46</f>
+        <v>2.1652173913043475E-3</v>
+      </c>
+      <c r="H18" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>8.6608695652173901E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="B19" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="20" t="s">
+      <c r="C19" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="5">
-        <v>1</v>
-      </c>
-      <c r="E19" s="20" t="s">
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
         <v>20</v>
       </c>
-      <c r="F19" s="21" t="s">
+      <c r="F19" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="19" t="s">
+      <c r="G19" s="21">
+        <f>0.0508/20</f>
+        <v>2.5399999999999997E-3</v>
+      </c>
+      <c r="H19" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>2.5399999999999997E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B20" s="20" t="s">
+      <c r="B20" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="20" t="s">
+      <c r="C20" t="s">
         <v>29</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20">
         <v>2</v>
       </c>
-      <c r="E20" s="20" t="s">
+      <c r="E20" t="s">
         <v>47</v>
       </c>
-      <c r="F20" s="21" t="s">
+      <c r="F20" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="19" t="s">
+      <c r="G20" s="21">
+        <f>0.2768/30</f>
+        <v>9.226666666666666E-3</v>
+      </c>
+      <c r="H20" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>1.8453333333333332E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B21" s="20" t="s">
+      <c r="B21" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="20" t="s">
+      <c r="C21" t="s">
         <v>50</v>
       </c>
-      <c r="D21" s="5">
+      <c r="D21">
         <v>8</v>
       </c>
-      <c r="E21" s="20" t="s">
+      <c r="E21" t="s">
         <v>52</v>
       </c>
-      <c r="F21" s="21" t="s">
+      <c r="F21" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="19" t="s">
+      <c r="G21" s="21">
+        <f>2.4027/88</f>
+        <v>2.730340909090909E-2</v>
+      </c>
+      <c r="H21" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>0.21842727272727272</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="20" t="s">
+      <c r="B22" t="s">
         <v>54</v>
       </c>
-      <c r="C22" s="20" t="s">
+      <c r="C22" t="s">
         <v>55</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D22">
         <v>12</v>
       </c>
-      <c r="E22" s="20" t="s">
+      <c r="E22" t="s">
         <v>57</v>
       </c>
-      <c r="F22" s="21" t="s">
+      <c r="F22" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="19" t="s">
+      <c r="G22" s="21">
+        <f>4.2963/124</f>
+        <v>3.464758064516129E-2</v>
+      </c>
+      <c r="H22" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>0.41577096774193545</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B23" s="20" t="s">
+      <c r="B23" t="s">
         <v>59</v>
       </c>
-      <c r="C23" s="20" t="s">
+      <c r="C23" t="s">
         <v>60</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D23">
         <v>2</v>
       </c>
-      <c r="E23" s="20" t="s">
+      <c r="E23" t="s">
         <v>61</v>
       </c>
-      <c r="F23" s="21" t="s">
+      <c r="F23" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="19" t="s">
+      <c r="G23" s="21">
+        <f>0.5062/28</f>
+        <v>1.8078571428571426E-2</v>
+      </c>
+      <c r="H23" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>3.6157142857142853E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B24" s="20" t="s">
+      <c r="B24" t="s">
         <v>63</v>
       </c>
-      <c r="C24" s="20" t="s">
+      <c r="C24" t="s">
         <v>64</v>
       </c>
-      <c r="D24" s="5">
+      <c r="D24">
         <v>2</v>
       </c>
-      <c r="E24" s="20" t="s">
+      <c r="E24" t="s">
         <v>65</v>
       </c>
-      <c r="F24" s="21" t="s">
+      <c r="F24" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="19" t="s">
+      <c r="G24" s="21">
+        <v>8.7400000000000005E-2</v>
+      </c>
+      <c r="H24" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>0.17480000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B25" s="20" t="s">
+      <c r="B25" t="s">
         <v>67</v>
       </c>
-      <c r="C25" s="20" t="s">
+      <c r="C25" t="s">
         <v>68</v>
       </c>
-      <c r="D25" s="5">
+      <c r="D25">
         <v>4</v>
       </c>
-      <c r="E25" s="20" t="s">
+      <c r="E25" t="s">
         <v>57</v>
       </c>
-      <c r="F25" s="21" t="s">
+      <c r="F25" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="19" t="s">
+      <c r="G25" s="21">
+        <f>0.4745/45</f>
+        <v>1.0544444444444443E-2</v>
+      </c>
+      <c r="H25" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>4.2177777777777772E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B26" s="20" t="s">
+      <c r="B26" t="s">
         <v>71</v>
       </c>
-      <c r="C26" s="20" t="s">
+      <c r="C26" t="s">
         <v>72</v>
       </c>
-      <c r="D26" s="5">
-        <v>1</v>
-      </c>
-      <c r="E26" s="20" t="s">
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26" t="s">
         <v>73</v>
       </c>
-      <c r="F26" s="21" t="s">
+      <c r="F26" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="19" t="s">
+      <c r="G26" s="21">
+        <v>0.55900000000000005</v>
+      </c>
+      <c r="H26" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>0.55900000000000005</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B27" s="20" t="s">
+      <c r="B27" t="s">
         <v>75</v>
       </c>
-      <c r="C27" s="20" t="s">
+      <c r="C27" t="s">
         <v>76</v>
       </c>
-      <c r="D27" s="5">
-        <v>1</v>
-      </c>
-      <c r="E27" s="20" t="s">
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27" t="s">
         <v>65</v>
       </c>
-      <c r="F27" s="21" t="s">
+      <c r="F27" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="19" t="s">
+      <c r="G27" s="21">
+        <f>0.6432/14</f>
+        <v>4.5942857142857139E-2</v>
+      </c>
+      <c r="H27" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>4.5942857142857139E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B28" s="20" t="s">
+      <c r="B28" t="s">
         <v>78</v>
       </c>
-      <c r="C28" s="20" t="s">
+      <c r="C28" t="s">
         <v>55</v>
       </c>
-      <c r="D28" s="5">
+      <c r="D28">
         <v>3</v>
       </c>
-      <c r="E28" s="20" t="s">
+      <c r="E28" t="s">
         <v>80</v>
       </c>
-      <c r="F28" s="21" t="s">
+      <c r="F28" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="19" t="s">
+      <c r="G28" s="21">
+        <f>2.1319/34</f>
+        <v>6.2702941176470586E-2</v>
+      </c>
+      <c r="H28" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>0.18810882352941177</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B29" s="20" t="s">
+      <c r="B29" t="s">
         <v>82</v>
       </c>
-      <c r="C29" s="20" t="s">
+      <c r="C29" t="s">
         <v>83</v>
       </c>
-      <c r="D29" s="5">
-        <v>1</v>
-      </c>
-      <c r="E29" s="20" t="s">
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29" t="s">
         <v>84</v>
       </c>
-      <c r="F29" s="21" t="s">
+      <c r="F29" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="19" t="s">
+      <c r="G29" s="21">
+        <f>5.6066/10</f>
+        <v>0.56066000000000005</v>
+      </c>
+      <c r="H29" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>0.56066000000000005</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B30" s="20" t="s">
+      <c r="B30" t="s">
         <v>86</v>
       </c>
-      <c r="C30" s="20" t="s">
+      <c r="C30" t="s">
         <v>87</v>
       </c>
-      <c r="D30" s="5">
-        <v>1</v>
-      </c>
-      <c r="E30" s="20" t="s">
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30" t="s">
         <v>88</v>
       </c>
-      <c r="F30" s="21" t="s">
+      <c r="F30" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="19" t="s">
+      <c r="G30" s="21">
+        <v>0.8196</v>
+      </c>
+      <c r="H30" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>0.8196</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B31" s="20" t="s">
+      <c r="B31" t="s">
         <v>90</v>
       </c>
-      <c r="C31" s="20" t="s">
+      <c r="C31" t="s">
         <v>91</v>
       </c>
-      <c r="D31" s="5">
-        <v>1</v>
-      </c>
-      <c r="E31" s="20" t="s">
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31" t="s">
         <v>10</v>
       </c>
-      <c r="F31" s="21" t="s">
+      <c r="F31" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="19" t="s">
+      <c r="G31" s="21">
+        <f>2.3971/10</f>
+        <v>0.23971000000000001</v>
+      </c>
+      <c r="H31" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>0.23971000000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B32" s="20" t="s">
+      <c r="B32" t="s">
         <v>94</v>
       </c>
-      <c r="C32" s="20" t="s">
+      <c r="C32" t="s">
         <v>95</v>
       </c>
-      <c r="D32" s="5">
-        <v>1</v>
-      </c>
-      <c r="E32" s="20" t="s">
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32" t="s">
         <v>97</v>
       </c>
-      <c r="F32" s="21" t="s">
+      <c r="F32" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="19" t="s">
+      <c r="G32" s="21">
+        <f>3.0222/10</f>
+        <v>0.30222000000000004</v>
+      </c>
+      <c r="H32" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>0.30222000000000004</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="B33" s="20" t="s">
+      <c r="B33" t="s">
         <v>99</v>
       </c>
-      <c r="C33" s="20" t="s">
+      <c r="C33" t="s">
         <v>100</v>
       </c>
-      <c r="D33" s="5">
-        <v>1</v>
-      </c>
-      <c r="E33" s="20" t="s">
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33" t="s">
         <v>10</v>
       </c>
-      <c r="F33" s="21" t="s">
+      <c r="F33" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="19" t="s">
+      <c r="G33" s="21">
+        <f>1.4895/10</f>
+        <v>0.14895</v>
+      </c>
+      <c r="H33" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>0.14895</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="B34" s="20" t="s">
+      <c r="B34" t="s">
         <v>103</v>
       </c>
-      <c r="C34" s="20" t="s">
+      <c r="C34" t="s">
         <v>104</v>
       </c>
-      <c r="D34" s="5">
-        <v>1</v>
-      </c>
-      <c r="E34" s="20" t="s">
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34" t="s">
         <v>10</v>
       </c>
-      <c r="F34" s="21" t="s">
+      <c r="F34" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="19" t="s">
+      <c r="G34" s="21">
+        <f>1.1547/10</f>
+        <v>0.11547</v>
+      </c>
+      <c r="H34" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>0.11547</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="B35" s="20" t="s">
+      <c r="B35" t="s">
         <v>107</v>
       </c>
-      <c r="C35" s="20" t="s">
+      <c r="C35" t="s">
         <v>108</v>
       </c>
-      <c r="D35" s="5">
-        <v>1</v>
-      </c>
-      <c r="E35" s="20" t="s">
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35" t="s">
         <v>10</v>
       </c>
-      <c r="F35" s="21" t="s">
+      <c r="F35" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="19" t="s">
+      <c r="G35" s="21">
+        <v>5.82</v>
+      </c>
+      <c r="H35" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>5.82</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="B36" s="20" t="s">
+      <c r="B36" t="s">
         <v>111</v>
       </c>
-      <c r="C36" s="20" t="s">
+      <c r="C36" t="s">
         <v>112</v>
       </c>
-      <c r="D36" s="5">
-        <v>1</v>
-      </c>
-      <c r="E36" s="20" t="s">
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36" t="s">
         <v>10</v>
       </c>
-      <c r="F36" s="21" t="s">
+      <c r="F36" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="19" t="s">
+      <c r="G36" s="21">
+        <f>0.7988/14</f>
+        <v>5.7057142857142855E-2</v>
+      </c>
+      <c r="H36" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>5.7057142857142855E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="B37" s="20" t="s">
+      <c r="B37" t="s">
         <v>115</v>
       </c>
-      <c r="C37" s="20" t="s">
+      <c r="C37" t="s">
         <v>116</v>
       </c>
-      <c r="D37" s="5">
+      <c r="D37">
         <v>4</v>
       </c>
-      <c r="E37" s="20" t="s">
+      <c r="E37" t="s">
         <v>117</v>
       </c>
-      <c r="F37" s="21" t="s">
+      <c r="F37" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="19" t="s">
+      <c r="G37" s="21">
+        <f>1.6488/44</f>
+        <v>3.7472727272727276E-2</v>
+      </c>
+      <c r="H37" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>0.1498909090909091</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="B38" s="20" t="s">
+      <c r="B38" t="s">
         <v>119</v>
       </c>
-      <c r="C38" s="20" t="s">
+      <c r="C38" t="s">
         <v>120</v>
       </c>
-      <c r="D38" s="5">
+      <c r="D38">
         <v>2</v>
       </c>
-      <c r="E38" s="20" t="s">
+      <c r="E38" t="s">
         <v>121</v>
       </c>
-      <c r="F38" s="21" t="s">
+      <c r="F38" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="19" t="s">
+      <c r="G38" s="21">
+        <f>0.6073/25</f>
+        <v>2.4291999999999998E-2</v>
+      </c>
+      <c r="H38" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>4.8583999999999995E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="B39" s="20" t="s">
+      <c r="B39" t="s">
         <v>123</v>
       </c>
-      <c r="C39" s="20" t="s">
+      <c r="C39" t="s">
         <v>120</v>
       </c>
-      <c r="D39" s="5">
+      <c r="D39">
         <v>2</v>
       </c>
-      <c r="E39" s="20" t="s">
+      <c r="E39" t="s">
         <v>124</v>
       </c>
-      <c r="F39" s="21" t="s">
+      <c r="F39" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="19" t="s">
+      <c r="G39" s="21">
+        <f>3.2595/20</f>
+        <v>0.16297500000000001</v>
+      </c>
+      <c r="H39" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>0.32595000000000002</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="B40" s="20" t="s">
+      <c r="B40" t="s">
         <v>126</v>
       </c>
-      <c r="C40" s="20" t="s">
+      <c r="C40" t="s">
         <v>120</v>
       </c>
-      <c r="D40" s="5">
-        <v>1</v>
-      </c>
-      <c r="E40" s="20" t="s">
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40" t="s">
         <v>73</v>
       </c>
-      <c r="F40" s="21" t="s">
+      <c r="F40" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="19" t="s">
+      <c r="G40" s="21">
+        <f>0.4392/15</f>
+        <v>2.9279999999999997E-2</v>
+      </c>
+      <c r="H40" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>2.9279999999999997E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="B41" s="20" t="s">
+      <c r="B41" t="s">
         <v>128</v>
       </c>
-      <c r="C41" s="20" t="s">
+      <c r="C41" t="s">
         <v>129</v>
       </c>
-      <c r="D41" s="5">
+      <c r="D41">
         <v>3</v>
       </c>
-      <c r="E41" s="20" t="s">
+      <c r="E41" t="s">
         <v>131</v>
       </c>
-      <c r="F41" s="21" t="s">
+      <c r="F41" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="19" t="s">
+      <c r="G41" s="21">
+        <f>0.0377/40</f>
+        <v>9.4249999999999998E-4</v>
+      </c>
+      <c r="H41" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>2.8275000000000002E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="B42" s="20" t="s">
+      <c r="B42" t="s">
         <v>133</v>
       </c>
-      <c r="C42" s="20" t="s">
+      <c r="C42" t="s">
         <v>129</v>
       </c>
-      <c r="D42" s="5">
-        <v>1</v>
-      </c>
-      <c r="E42" s="20" t="s">
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42" t="s">
         <v>135</v>
       </c>
-      <c r="F42" s="21" t="s">
+      <c r="F42" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="19" t="s">
+      <c r="G42" s="21">
+        <f>0.0188/20</f>
+        <v>9.4000000000000008E-4</v>
+      </c>
+      <c r="H42" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>9.4000000000000008E-4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="B43" s="20" t="s">
+      <c r="B43" t="s">
         <v>137</v>
       </c>
-      <c r="C43" s="20" t="s">
+      <c r="C43" t="s">
         <v>129</v>
       </c>
-      <c r="D43" s="5">
+      <c r="D43">
         <v>11</v>
       </c>
-      <c r="E43" s="20" t="s">
+      <c r="E43" t="s">
         <v>131</v>
       </c>
-      <c r="F43" s="21" t="s">
+      <c r="F43" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="19" t="s">
+      <c r="G43" s="21">
+        <f>0.113/100</f>
+        <v>1.1299999999999999E-3</v>
+      </c>
+      <c r="H43" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>1.243E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="B44" s="20" t="s">
+      <c r="B44" t="s">
         <v>140</v>
       </c>
-      <c r="C44" s="20" t="s">
+      <c r="C44" t="s">
         <v>129</v>
       </c>
-      <c r="D44" s="5">
-        <v>1</v>
-      </c>
-      <c r="E44" s="20" t="s">
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44" t="s">
         <v>80</v>
       </c>
-      <c r="F44" s="21" t="s">
+      <c r="F44" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="19" t="s">
+      <c r="G44" s="21">
+        <f>0.0207/20</f>
+        <v>1.0349999999999999E-3</v>
+      </c>
+      <c r="H44" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>1.0349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="B45" s="20" t="s">
+      <c r="B45" t="s">
         <v>143</v>
       </c>
-      <c r="C45" s="20" t="s">
+      <c r="C45" t="s">
         <v>129</v>
       </c>
-      <c r="D45" s="5">
+      <c r="D45">
         <v>18</v>
       </c>
-      <c r="E45" s="20" t="s">
+      <c r="E45" t="s">
         <v>131</v>
       </c>
-      <c r="F45" s="21" t="s">
+      <c r="F45" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="19" t="s">
+      <c r="G45" s="21">
+        <f>0.1864/220</f>
+        <v>8.4727272727272733E-4</v>
+      </c>
+      <c r="H45" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>1.5250909090909093E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="B46" s="20" t="s">
+      <c r="B46" t="s">
         <v>146</v>
       </c>
-      <c r="C46" s="20" t="s">
+      <c r="C46" t="s">
         <v>129</v>
       </c>
-      <c r="D46" s="5">
-        <v>1</v>
-      </c>
-      <c r="E46" s="20" t="s">
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46" t="s">
         <v>131</v>
       </c>
-      <c r="F46" s="21" t="s">
+      <c r="F46" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="19" t="s">
+      <c r="G46" s="21">
+        <f>0.0188/20</f>
+        <v>9.4000000000000008E-4</v>
+      </c>
+      <c r="H46" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>9.4000000000000008E-4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="B47" s="20" t="s">
+      <c r="B47" t="s">
         <v>149</v>
       </c>
-      <c r="C47" s="20" t="s">
+      <c r="C47" t="s">
         <v>129</v>
       </c>
-      <c r="D47" s="5">
+      <c r="D47">
         <v>3</v>
       </c>
-      <c r="E47" s="20" t="s">
+      <c r="E47" t="s">
         <v>131</v>
       </c>
-      <c r="F47" s="21" t="s">
+      <c r="F47" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="19" t="s">
+      <c r="G47" s="21">
+        <f>0.0377/40</f>
+        <v>9.4249999999999998E-4</v>
+      </c>
+      <c r="H47" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>2.8275000000000002E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="B48" s="20" t="s">
+      <c r="B48" t="s">
         <v>152</v>
       </c>
-      <c r="C48" s="20" t="s">
+      <c r="C48" t="s">
         <v>129</v>
       </c>
-      <c r="D48" s="5">
+      <c r="D48">
         <v>3</v>
       </c>
-      <c r="E48" s="20" t="s">
+      <c r="E48" t="s">
         <v>131</v>
       </c>
-      <c r="F48" s="21" t="s">
+      <c r="F48" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="19" t="s">
+      <c r="G48" s="21">
+        <f>0.1864/220</f>
+        <v>8.4727272727272733E-4</v>
+      </c>
+      <c r="H48" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>2.541818181818182E-3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="B49" s="20" t="s">
+      <c r="B49" t="s">
         <v>154</v>
       </c>
-      <c r="C49" s="20" t="s">
+      <c r="C49" t="s">
         <v>129</v>
       </c>
-      <c r="D49" s="5">
+      <c r="D49">
         <v>4</v>
       </c>
-      <c r="E49" s="20" t="s">
+      <c r="E49" t="s">
         <v>156</v>
       </c>
-      <c r="F49" s="21" t="s">
+      <c r="F49" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="19" t="s">
+      <c r="G49" s="21">
+        <f>0.0471/50</f>
+        <v>9.4200000000000002E-4</v>
+      </c>
+      <c r="H49" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>3.7680000000000001E-3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="B50" s="20" t="s">
+      <c r="B50" t="s">
         <v>158</v>
       </c>
-      <c r="C50" s="20" t="s">
+      <c r="C50" t="s">
         <v>129</v>
       </c>
-      <c r="D50" s="5">
+      <c r="D50">
         <v>32</v>
       </c>
-      <c r="E50" s="20" t="s">
+      <c r="E50" t="s">
         <v>131</v>
       </c>
-      <c r="F50" s="21" t="s">
+      <c r="F50" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="19" t="s">
+      <c r="G50" s="21">
+        <f>0.3107/330</f>
+        <v>9.4151515151515142E-4</v>
+      </c>
+      <c r="H50" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>3.0128484848484845E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="B51" s="20" t="s">
+      <c r="B51" t="s">
         <v>161</v>
       </c>
-      <c r="C51" s="20" t="s">
+      <c r="C51" t="s">
         <v>129</v>
       </c>
-      <c r="D51" s="5">
-        <v>1</v>
-      </c>
-      <c r="E51" s="20" t="s">
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51" t="s">
         <v>156</v>
       </c>
-      <c r="F51" s="21" t="s">
+      <c r="F51" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="19" t="s">
+      <c r="G51" s="21">
+        <f>0.0226/20</f>
+        <v>1.1299999999999999E-3</v>
+      </c>
+      <c r="H51" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>1.1299999999999999E-3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="B52" s="20" t="s">
+      <c r="B52" t="s">
         <v>164</v>
       </c>
-      <c r="C52" s="20" t="s">
+      <c r="C52" t="s">
         <v>129</v>
       </c>
-      <c r="D52" s="5">
-        <v>1</v>
-      </c>
-      <c r="E52" s="20" t="s">
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="E52" t="s">
         <v>135</v>
       </c>
-      <c r="F52" s="21" t="s">
+      <c r="F52" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="19" t="s">
+      <c r="G52" s="21">
+        <f>0.0188/20</f>
+        <v>9.4000000000000008E-4</v>
+      </c>
+      <c r="H52" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>9.4000000000000008E-4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="B53" s="20" t="s">
+      <c r="B53" t="s">
         <v>167</v>
       </c>
-      <c r="C53" s="20" t="s">
+      <c r="C53" t="s">
         <v>129</v>
       </c>
-      <c r="D53" s="5">
-        <v>1</v>
-      </c>
-      <c r="E53" s="20" t="s">
+      <c r="D53">
+        <v>1</v>
+      </c>
+      <c r="E53" t="s">
         <v>131</v>
       </c>
-      <c r="F53" s="21" t="s">
+      <c r="F53" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="19" t="s">
+      <c r="G53" s="21">
+        <f>0.0188/20</f>
+        <v>9.4000000000000008E-4</v>
+      </c>
+      <c r="H53" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>9.4000000000000008E-4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="B54" s="20" t="s">
+      <c r="B54" t="s">
         <v>170</v>
       </c>
-      <c r="C54" s="20" t="s">
+      <c r="C54" t="s">
         <v>129</v>
       </c>
-      <c r="D54" s="5">
+      <c r="D54">
         <v>9</v>
       </c>
-      <c r="E54" s="20" t="s">
+      <c r="E54" t="s">
         <v>80</v>
       </c>
-      <c r="F54" s="21" t="s">
+      <c r="F54" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="19" t="s">
+      <c r="G54" s="21">
+        <f>0.0942/100</f>
+        <v>9.4200000000000002E-4</v>
+      </c>
+      <c r="H54" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>8.4779999999999994E-3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="B55" s="20" t="s">
+      <c r="B55" t="s">
         <v>173</v>
       </c>
-      <c r="C55" s="20" t="s">
+      <c r="C55" t="s">
         <v>129</v>
       </c>
-      <c r="D55" s="5">
-        <v>1</v>
-      </c>
-      <c r="E55" s="20" t="s">
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="E55" t="s">
         <v>175</v>
       </c>
-      <c r="F55" s="21" t="s">
+      <c r="F55" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="19" t="s">
+      <c r="G55" s="21">
+        <f>0.0188/20</f>
+        <v>9.4000000000000008E-4</v>
+      </c>
+      <c r="H55" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>9.4000000000000008E-4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="B56" s="20" t="s">
+      <c r="B56" t="s">
         <v>177</v>
       </c>
-      <c r="C56" s="20" t="s">
+      <c r="C56" t="s">
         <v>129</v>
       </c>
-      <c r="D56" s="5">
-        <v>1</v>
-      </c>
-      <c r="E56" s="20" t="s">
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56" t="s">
         <v>135</v>
       </c>
-      <c r="F56" s="21" t="s">
+      <c r="F56" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="19" t="s">
+      <c r="G56" s="21">
+        <f>0.0188/20</f>
+        <v>9.4000000000000008E-4</v>
+      </c>
+      <c r="H56" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>9.4000000000000008E-4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="B57" s="20" t="s">
+      <c r="B57" t="s">
         <v>180</v>
       </c>
-      <c r="C57" s="20" t="s">
+      <c r="C57" t="s">
         <v>129</v>
       </c>
-      <c r="D57" s="5">
-        <v>1</v>
-      </c>
-      <c r="E57" s="20" t="s">
+      <c r="D57">
+        <v>1</v>
+      </c>
+      <c r="E57" t="s">
         <v>182</v>
       </c>
-      <c r="F57" s="21" t="s">
+      <c r="F57" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="19" t="s">
+      <c r="G57" s="21">
+        <f>0.0188/20</f>
+        <v>9.4000000000000008E-4</v>
+      </c>
+      <c r="H57" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>9.4000000000000008E-4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="B58" s="20" t="s">
+      <c r="B58" t="s">
         <v>184</v>
       </c>
-      <c r="C58" s="20" t="s">
+      <c r="C58" t="s">
         <v>185</v>
       </c>
-      <c r="D58" s="5">
-        <v>1</v>
-      </c>
-      <c r="E58" s="20" t="s">
+      <c r="D58">
+        <v>1</v>
+      </c>
+      <c r="E58" t="s">
         <v>10</v>
       </c>
-      <c r="F58" s="21" t="s">
+      <c r="F58" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="19" t="s">
+      <c r="G58" s="21">
+        <f>5.536/10</f>
+        <v>0.55359999999999998</v>
+      </c>
+      <c r="H58" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>0.55359999999999998</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="B59" s="20" t="s">
+      <c r="B59" t="s">
         <v>188</v>
       </c>
-      <c r="C59" s="20" t="s">
+      <c r="C59" t="s">
         <v>129</v>
       </c>
-      <c r="D59" s="5">
-        <v>1</v>
-      </c>
-      <c r="E59" s="20" t="s">
+      <c r="D59">
+        <v>1</v>
+      </c>
+      <c r="E59" t="s">
         <v>84</v>
       </c>
-      <c r="F59" s="21" t="s">
+      <c r="F59" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="19" t="s">
+      <c r="G59" s="21">
+        <f>0.696/14</f>
+        <v>4.9714285714285711E-2</v>
+      </c>
+      <c r="H59" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>4.9714285714285711E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="B60" s="20" t="s">
+      <c r="B60" t="s">
         <v>191</v>
       </c>
-      <c r="C60" s="20" t="s">
+      <c r="C60" t="s">
         <v>192</v>
       </c>
-      <c r="D60" s="5">
-        <v>1</v>
-      </c>
-      <c r="E60" s="20" t="s">
+      <c r="D60">
+        <v>1</v>
+      </c>
+      <c r="E60" t="s">
         <v>193</v>
       </c>
-      <c r="F60" s="21" t="s">
+      <c r="F60" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="19" t="s">
+      <c r="G60" s="21">
+        <f>2.1852/10</f>
+        <v>0.21851999999999999</v>
+      </c>
+      <c r="H60" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>0.21851999999999999</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="B61" s="20" t="s">
+      <c r="B61" t="s">
         <v>195</v>
       </c>
-      <c r="C61" s="20" t="s">
+      <c r="C61" t="s">
         <v>196</v>
       </c>
-      <c r="D61" s="5">
-        <v>1</v>
-      </c>
-      <c r="E61" s="20" t="s">
+      <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="E61" t="s">
         <v>198</v>
       </c>
-      <c r="F61" s="21" t="s">
+      <c r="F61" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="19" t="s">
+      <c r="G61" s="21">
+        <v>1.746</v>
+      </c>
+      <c r="H61" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>1.746</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="B62" s="20" t="s">
+      <c r="B62" t="s">
         <v>200</v>
       </c>
-      <c r="C62" s="20" t="s">
+      <c r="C62" t="s">
         <v>201</v>
       </c>
-      <c r="D62" s="5">
-        <v>1</v>
-      </c>
-      <c r="E62" s="20" t="s">
+      <c r="D62">
+        <v>1</v>
+      </c>
+      <c r="E62" t="s">
         <v>202</v>
       </c>
-      <c r="F62" s="21" t="s">
+      <c r="F62" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="19" t="s">
+      <c r="G62" s="21">
+        <v>1.353</v>
+      </c>
+      <c r="H62" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>1.353</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="B63" s="20" t="s">
+      <c r="B63" t="s">
         <v>204</v>
       </c>
-      <c r="C63" s="20" t="s">
+      <c r="C63" t="s">
         <v>205</v>
       </c>
-      <c r="D63" s="5">
-        <v>1</v>
-      </c>
-      <c r="E63" s="20" t="s">
+      <c r="D63">
+        <v>1</v>
+      </c>
+      <c r="E63" t="s">
         <v>206</v>
       </c>
-      <c r="F63" s="21" t="s">
+      <c r="F63" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="19" t="s">
+      <c r="G63" s="21">
+        <f>2.1852/10</f>
+        <v>0.21851999999999999</v>
+      </c>
+      <c r="H63" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>0.21851999999999999</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="B64" s="20" t="s">
+      <c r="B64" t="s">
         <v>208</v>
       </c>
-      <c r="C64" s="20" t="s">
+      <c r="C64" t="s">
         <v>209</v>
       </c>
-      <c r="D64" s="5">
-        <v>1</v>
-      </c>
-      <c r="E64" s="20" t="s">
+      <c r="D64">
+        <v>1</v>
+      </c>
+      <c r="E64" t="s">
         <v>210</v>
       </c>
-      <c r="F64" s="21" t="s">
+      <c r="F64" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="19" t="s">
+      <c r="G64" s="21">
+        <f>17.0741/10</f>
+        <v>1.7074100000000001</v>
+      </c>
+      <c r="H64" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>1.7074100000000001</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="B65" s="20" t="s">
+      <c r="B65" t="s">
         <v>212</v>
       </c>
-      <c r="C65" s="20" t="s">
+      <c r="C65" t="s">
         <v>213</v>
       </c>
-      <c r="D65" s="5">
-        <v>1</v>
-      </c>
-      <c r="E65" s="20" t="s">
+      <c r="D65">
+        <v>1</v>
+      </c>
+      <c r="E65" t="s">
         <v>215</v>
       </c>
-      <c r="F65" s="21" t="s">
+      <c r="F65" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="19" t="s">
+      <c r="G65" s="21">
+        <f>41.5202/10</f>
+        <v>4.1520200000000003</v>
+      </c>
+      <c r="H65" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>4.1520200000000003</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="B66" s="20" t="s">
+      <c r="B66" t="s">
         <v>217</v>
       </c>
-      <c r="C66" s="20" t="s">
+      <c r="C66" t="s">
         <v>218</v>
       </c>
-      <c r="D66" s="5">
-        <v>1</v>
-      </c>
-      <c r="E66" s="20" t="s">
+      <c r="D66">
+        <v>1</v>
+      </c>
+      <c r="E66" t="s">
         <v>198</v>
       </c>
-      <c r="F66" s="21" t="s">
+      <c r="F66" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="19" t="s">
+      <c r="G66" s="21">
+        <f>7.5838/10</f>
+        <v>0.75838000000000005</v>
+      </c>
+      <c r="H66" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>0.75838000000000005</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="B67" s="20" t="s">
+      <c r="B67" t="s">
         <v>220</v>
       </c>
-      <c r="C67" s="20" t="s">
+      <c r="C67" t="s">
         <v>221</v>
       </c>
-      <c r="D67" s="5">
-        <v>1</v>
-      </c>
-      <c r="E67" s="20" t="s">
+      <c r="D67">
+        <v>1</v>
+      </c>
+      <c r="E67" t="s">
         <v>222</v>
       </c>
-      <c r="F67" s="21" t="s">
+      <c r="F67" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="19" t="s">
+      <c r="G67" s="21">
+        <f>14.2496/10</f>
+        <v>1.42496</v>
+      </c>
+      <c r="H67" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>1.42496</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="B68" s="20" t="s">
+      <c r="B68" t="s">
         <v>224</v>
       </c>
-      <c r="C68" s="20" t="s">
+      <c r="C68" t="s">
         <v>225</v>
       </c>
-      <c r="D68" s="5">
-        <v>1</v>
-      </c>
-      <c r="E68" s="20" t="s">
+      <c r="D68">
+        <v>1</v>
+      </c>
+      <c r="E68" t="s">
         <v>193</v>
       </c>
-      <c r="F68" s="21" t="s">
+      <c r="F68" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="19" t="s">
+      <c r="G68" s="21">
+        <f>4.5757/10</f>
+        <v>0.45757000000000003</v>
+      </c>
+      <c r="H68" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>0.45757000000000003</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="B69" s="20" t="s">
+      <c r="B69" t="s">
         <v>228</v>
       </c>
-      <c r="C69" s="20" t="s">
+      <c r="C69" t="s">
         <v>229</v>
       </c>
-      <c r="D69" s="5">
-        <v>1</v>
-      </c>
-      <c r="E69" s="20" t="s">
+      <c r="D69">
+        <v>1</v>
+      </c>
+      <c r="E69" t="s">
         <v>198</v>
       </c>
-      <c r="F69" s="21" t="s">
+      <c r="F69" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="19" t="s">
+      <c r="G69" s="21">
+        <v>6.9850000000000003</v>
+      </c>
+      <c r="H69" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>6.9850000000000003</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="B70" s="20" t="s">
+      <c r="B70" t="s">
         <v>232</v>
       </c>
-      <c r="C70" s="20" t="s">
+      <c r="C70" t="s">
         <v>233</v>
       </c>
-      <c r="D70" s="5">
-        <v>1</v>
-      </c>
-      <c r="E70" s="20" t="s">
+      <c r="D70">
+        <v>1</v>
+      </c>
+      <c r="E70" t="s">
         <v>234</v>
       </c>
-      <c r="F70" s="21" t="s">
+      <c r="F70" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="19" t="s">
+      <c r="G70" s="21">
+        <f>2.3556/10</f>
+        <v>0.23555999999999999</v>
+      </c>
+      <c r="H70" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>0.23555999999999999</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="B71" s="20" t="s">
+      <c r="B71" t="s">
         <v>236</v>
       </c>
-      <c r="C71" s="20" t="s">
+      <c r="C71" t="s">
         <v>237</v>
       </c>
-      <c r="D71" s="5">
-        <v>1</v>
-      </c>
-      <c r="E71" s="20" t="s">
+      <c r="D71">
+        <v>1</v>
+      </c>
+      <c r="E71" t="s">
         <v>193</v>
       </c>
-      <c r="F71" s="21" t="s">
+      <c r="F71" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="19" t="s">
+      <c r="G71" s="21">
+        <v>1.0469999999999999</v>
+      </c>
+      <c r="H71" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>1.0469999999999999</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="B72" s="20" t="s">
+      <c r="B72" t="s">
         <v>240</v>
       </c>
-      <c r="C72" s="20" t="s">
+      <c r="C72" t="s">
         <v>205</v>
       </c>
-      <c r="D72" s="5">
-        <v>1</v>
-      </c>
-      <c r="E72" s="20" t="s">
+      <c r="D72">
+        <v>1</v>
+      </c>
+      <c r="E72" t="s">
         <v>193</v>
       </c>
-      <c r="F72" s="21" t="s">
+      <c r="F72" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="22" t="s">
+      <c r="G72" s="21">
+        <v>0.94599999999999995</v>
+      </c>
+      <c r="H72" s="22">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>0.94599999999999995</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="6" t="s">
         <v>241</v>
       </c>
-      <c r="B73" s="23" t="s">
+      <c r="B73" s="7" t="s">
         <v>242</v>
       </c>
-      <c r="C73" s="23" t="s">
+      <c r="C73" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="D73" s="8">
-        <v>1</v>
-      </c>
-      <c r="E73" s="23" t="s">
+      <c r="D73" s="7">
+        <v>1</v>
+      </c>
+      <c r="E73" s="7" t="s">
         <v>245</v>
       </c>
-      <c r="F73" s="24" t="s">
+      <c r="F73" s="7" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="G73" s="7">
+        <v>0.436</v>
+      </c>
+      <c r="H73" s="23">
+        <f>BOM___AnthC_M2_R4[[#This Row],[Unit Price]]*BOM___AnthC_M2_R4[[#This Row],[Qty]]</f>
+        <v>0.436</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="21.75" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="F74" s="14" t="s">
+        <v>252</v>
+      </c>
+      <c r="H74" s="14">
+        <f>SUM(H10:H73)</f>
+        <v>36.242552487315642</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:B2"/>

</xml_diff>